<commit_message>
add emission lines tables
</commit_message>
<xml_diff>
--- a/StudyFors2SED/GalEmissionLines.xlsx
+++ b/StudyFors2SED/GalEmissionLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagoret/MacOSX/GitHub/LSST/PhotoZ_PhD/StudyFors2SED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AAFF5F-10F8-BA4C-A925-47E52DDACC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B537692E-348D-4E4E-B949-47E207BB5C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16720" xr2:uid="{5C4A1DCC-B10E-644A-9FC0-CB82453AB3D3}"/>
+    <workbookView xWindow="20" yWindow="1280" windowWidth="28040" windowHeight="16720" xr2:uid="{5C4A1DCC-B10E-644A-9FC0-CB82453AB3D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -11287,8 +11287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2BD5F4-CC47-D340-9A6D-811B5AF46E76}">
   <dimension ref="A1:K235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>